<commit_message>
casi terminada faltan pruebas
</commit_message>
<xml_diff>
--- a/Practica1/reporte_200915609.xlsx
+++ b/Practica1/reporte_200915609.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Nombre</t>
   </si>
@@ -45,40 +45,109 @@
     <t>Tipo(extension)</t>
   </si>
   <si>
-    <t>Main.xaml</t>
-  </si>
-  <si>
-    <t>project.json</t>
-  </si>
-  <si>
-    <t>C:\Users\gjoan\Desktop\IA\LABORATORIO\PRACTICA 1\P1_IA\Practica1</t>
-  </si>
-  <si>
-    <t>25/01/2021 05:06:54</t>
-  </si>
-  <si>
-    <t>25/01/2021 08:30:13</t>
-  </si>
-  <si>
-    <t>.xaml</t>
-  </si>
-  <si>
-    <t>25/01/2021 08:30:11</t>
-  </si>
-  <si>
-    <t>.json</t>
-  </si>
-  <si>
-    <t>reporte_200915609.xlsx</t>
-  </si>
-  <si>
-    <t>25/01/2021 05:50:19</t>
-  </si>
-  <si>
-    <t>25/01/2021 08:30:25</t>
+    <t>F:\Descargas\ExcelReadWrite\ExcelReadWrite</t>
+  </si>
+  <si>
+    <t>24/11/2020 08:29:44</t>
+  </si>
+  <si>
+    <t>ExcelReadWrite.suo</t>
+  </si>
+  <si>
+    <t>ExcelReadWrite.xlsx</t>
+  </si>
+  <si>
+    <t>ExcelWriteStep.cs</t>
+  </si>
+  <si>
+    <t>.cs</t>
+  </si>
+  <si>
+    <t>.suo</t>
   </si>
   <si>
     <t>.xlsx</t>
+  </si>
+  <si>
+    <t>Guía de Aprendizaje Ciencia y Medición.docx</t>
+  </si>
+  <si>
+    <t>C:\Users\gjoan\Desktop\QUIMICA</t>
+  </si>
+  <si>
+    <t>20/01/2021 05:52:53</t>
+  </si>
+  <si>
+    <t>21/01/2021 12:04:32</t>
+  </si>
+  <si>
+    <t>.docx</t>
+  </si>
+  <si>
+    <t>Material de apoyo unidad I.pdf</t>
+  </si>
+  <si>
+    <t>21/01/2021 12:04:07</t>
+  </si>
+  <si>
+    <t>.pdf</t>
+  </si>
+  <si>
+    <t>Medición y Cifras Significativas.pdf</t>
+  </si>
+  <si>
+    <t>21/01/2021 12:05:47</t>
+  </si>
+  <si>
+    <t>21/01/2021 12:12:28</t>
+  </si>
+  <si>
+    <t>NORMA COGUANOR_NGO_4_010_2a._Revision.pdf</t>
+  </si>
+  <si>
+    <t>21/01/2021 12:06:18</t>
+  </si>
+  <si>
+    <t>21/01/2021 09:07:02</t>
+  </si>
+  <si>
+    <t>Nueva imagen de mapa de bits.bmp</t>
+  </si>
+  <si>
+    <t>28/01/2021 10:52:33</t>
+  </si>
+  <si>
+    <t>28/01/2021 10:53:33</t>
+  </si>
+  <si>
+    <t>.bmp</t>
+  </si>
+  <si>
+    <t>Nuevo documento de texto.txt</t>
+  </si>
+  <si>
+    <t>28/01/2021 10:52:25</t>
+  </si>
+  <si>
+    <t>28/01/2021 10:52:36</t>
+  </si>
+  <si>
+    <t>.txt</t>
+  </si>
+  <si>
+    <t>TABLA DE CONVERSIÓN DE UNIDADES.pdf</t>
+  </si>
+  <si>
+    <t>21/01/2021 08:52:56</t>
+  </si>
+  <si>
+    <t>23/01/2021 07:22:04</t>
+  </si>
+  <si>
+    <t>Tarea Preparatoria Primer Parcial.pdf</t>
+  </si>
+  <si>
+    <t>23/01/2021 07:05:59</t>
   </si>
 </sst>
 </file>
@@ -114,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -424,62 +494,222 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>20348</v>
+        <v>24777</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>1388</v>
+        <v>259760</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>8895</v>
+        <v>339523</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>503289</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>26028</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>473194</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
+      <c r="B10">
+        <v>20992</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43620.19122685185</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>9477</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43620.19122685185</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>6238</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43620.19122685185</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>